<commit_message>
Updated to Fit New Requirements
</commit_message>
<xml_diff>
--- a/Data/Config/Config.xlsx
+++ b/Data/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nourshoreibah/Documents/UiPath/AutoSamirRayanDispatcher/Data/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6F7480-C5F9-8349-A886-6F93FC9EA90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA77F94-2CE4-E54A-8712-7543F4BAF9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{936A213D-1EC4-6645-8964-F191FCC7D657}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Key</t>
   </si>
@@ -68,13 +68,67 @@
   </si>
   <si>
     <t>https://www.auto-samirrayan.com/new-cars</t>
+  </si>
+  <si>
+    <t>msgLoading</t>
+  </si>
+  <si>
+    <t>msgBadAttachments</t>
+  </si>
+  <si>
+    <t>ValidBrands</t>
+  </si>
+  <si>
+    <t>msgNSheets</t>
+  </si>
+  <si>
+    <t>msgSheetFormat</t>
+  </si>
+  <si>
+    <t>Found workbook that does not contain exactly one sheet. Sending email</t>
+  </si>
+  <si>
+    <t>Foud email with incorrect attachments. Sending email</t>
+  </si>
+  <si>
+    <t>There was an error loading a page. Please try again or contact administrator for help</t>
+  </si>
+  <si>
+    <t>Excel sheet must contain exactly one column called "BRAND NAME" with at least 1 brand</t>
+  </si>
+  <si>
+    <t>msgInvComp</t>
+  </si>
+  <si>
+    <t>One or more companies in the provided Excel sheet are invalid</t>
+  </si>
+  <si>
+    <t>msgEmailFailure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There was an error reading your inbox. Here is the error: </t>
+  </si>
+  <si>
+    <t>msgNoEmail</t>
+  </si>
+  <si>
+    <t>No Emails to Process</t>
+  </si>
+  <si>
+    <t>Mercedes,Opel,Chevrolet,Fiat,Jac,Kia,Nissan,Toyota,Audi,BMW,Peugeot,Ssang Yong,Skoda,suzuki,Seat,Chery,Hyundai,Alfa Romeo,Porche,BYD,Jaguar,MG,Jeep,Jetour,DS,Citroen,Subaru,Changan,Land Rover,Mini,Lexus,Haval,Forthing,Honda,ford,lada,maserati,Mitsubishi,Renault,Volkswagen,Volvo,BAIC,Bestune,GEELY,DFM,Cupra,Souedast</t>
+  </si>
+  <si>
+    <t>EmailSignature</t>
+  </si>
+  <si>
+    <t>Nour (RPA Team)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,7 +144,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="30"/>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFA31515"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -98,7 +166,7 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="24"/>
       <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -124,13 +192,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -466,56 +535,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C189C4E5-5312-834D-8D09-B96B1EAE3CAE}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="32" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
-    <col min="2" max="2" width="47.5" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="47.5" style="3" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="39" x14ac:dyDescent="0.45">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="39" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="39" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="39" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="27" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -531,7 +617,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="27" x14ac:dyDescent="0.35"/>
@@ -562,10 +648,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C8A495-658E-D242-A5BD-601EB7F27401}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -578,6 +664,62 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add more error messages
</commit_message>
<xml_diff>
--- a/Data/Config/Config.xlsx
+++ b/Data/Config/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nourshoreibah/Documents/UiPath/AutoSamirRayanDispatcher/Data/Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA77F94-2CE4-E54A-8712-7543F4BAF9C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1028EB8-4DF3-634D-BD3B-17AB4D97D703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" xr2:uid="{936A213D-1EC4-6645-8964-F191FCC7D657}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20080" activeTab="2" xr2:uid="{936A213D-1EC4-6645-8964-F191FCC7D657}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -73,9 +73,6 @@
     <t>msgLoading</t>
   </si>
   <si>
-    <t>msgBadAttachments</t>
-  </si>
-  <si>
     <t>ValidBrands</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>Found workbook that does not contain exactly one sheet. Sending email</t>
   </si>
   <si>
-    <t>Foud email with incorrect attachments. Sending email</t>
-  </si>
-  <si>
     <t>There was an error loading a page. Please try again or contact administrator for help</t>
   </si>
   <si>
@@ -122,6 +116,12 @@
   </si>
   <si>
     <t>Nour (RPA Team)</t>
+  </si>
+  <si>
+    <t>msgBadAttachment</t>
+  </si>
+  <si>
+    <t>Email does not contain exactly one xlsx file</t>
   </si>
 </sst>
 </file>
@@ -537,7 +537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C189C4E5-5312-834D-8D09-B96B1EAE3CAE}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -590,18 +590,18 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -650,8 +650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49C8A495-658E-D242-A5BD-601EB7F27401}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,55 +669,55 @@
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>